<commit_message>
added hw2 and start of hw3
</commit_message>
<xml_diff>
--- a/hw/hw2/hw2_algorithm_testing.xlsx
+++ b/hw/hw2/hw2_algorithm_testing.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zackmcnulty/Desktop/CSE/417/hw/hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B6B46-6C26-1549-9617-B79A30208825}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237184BE-1239-8B4D-89F9-734CDB1939A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{655B9E93-3D61-2645-88BB-75B84C8FC629}"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{655B9E93-3D61-2645-88BB-75B84C8FC629}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$B$2:$B$64</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$D$2:$D$64</definedName>
+    <definedName name="output_big" localSheetId="0">Sheet2!$A$65:$D$73</definedName>
     <definedName name="test_results" localSheetId="0">Sheet2!$A$2:$D$64</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -37,7 +36,18 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{C0734B9C-E119-B745-8D91-723701C7823D}" name="test_results" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{9EA78852-3A79-294C-A856-037EB837BE7F}" name="output_big" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/zackmcnulty/Desktop/CSE/417/hw/hw2/output_big.txt" space="1" consecutive="1">
+      <textFields count="5">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{C0734B9C-E119-B745-8D91-723701C7823D}" name="test_results" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/zackmcnulty/Desktop/CSE/417/hw/hw2/test_results.txt" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
@@ -52,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>nodes</t>
   </si>
@@ -253,6 +263,33 @@
   </si>
   <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>bigs/n2048d12s4.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d12s5.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d12s6.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d3s1.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d3s2.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d3s3.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d45s7.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d45s8.txt</t>
+  </si>
+  <si>
+    <t>bigs/n2048d45s9.txt</t>
   </si>
 </sst>
 </file>
@@ -446,10 +483,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$64</c:f>
+              <c:f>Sheet2!$B$2:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -638,16 +675,43 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$64</c:f>
+              <c:f>Sheet2!$D$2:$D$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>4.1021108627319301E-2</c:v>
                 </c:pt>
@@ -836,6 +900,33 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>5.3620338439941395E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.7985086441039997E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.7384986877441399E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.60550880432128E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.20820999145507E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1244058609008701E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0188102722167899E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.13002896308898901</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.13641691207885701</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.133769035339355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,10 +1445,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$64</c:f>
+              <c:f>Sheet2!$C$2:$C$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>31406</c:v>
                 </c:pt>
@@ -1546,16 +1637,43 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24576</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>24352</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>24280</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6130</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6174</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6170</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>90546</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>89128</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>88097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$64</c:f>
+              <c:f>Sheet2!$D$2:$D$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>4.1021108627319301E-2</c:v>
                 </c:pt>
@@ -1744,6 +1862,33 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>5.3620338439941395E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.7985086441039997E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.7384986877441399E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.60550880432128E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.20820999145507E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1244058609008701E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0188102722167899E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.13002896308898901</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.13641691207885701</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.133769035339355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3259,7 +3404,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test_results" connectionId="1" xr16:uid="{704C16CB-94F8-E549-B972-16581D9B5AD3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="output_big" connectionId="1" xr16:uid="{E6D471A8-7DC2-7B4D-B82C-84DF0C7FF27E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test_results" connectionId="2" xr16:uid="{704C16CB-94F8-E549-B972-16581D9B5AD3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3559,15 +3708,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEB0E3-6FED-A94F-B518-DE0487B45B0A}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -4467,6 +4616,132 @@
       </c>
       <c r="D64">
         <v>5.3620338439941395E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65">
+        <v>2048</v>
+      </c>
+      <c r="C65">
+        <v>24576</v>
+      </c>
+      <c r="D65">
+        <v>3.7985086441039997E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66">
+        <v>2048</v>
+      </c>
+      <c r="C66">
+        <v>24352</v>
+      </c>
+      <c r="D66">
+        <v>3.7384986877441399E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67">
+        <v>2048</v>
+      </c>
+      <c r="C67">
+        <v>24280</v>
+      </c>
+      <c r="D67">
+        <v>3.60550880432128E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68">
+        <v>2048</v>
+      </c>
+      <c r="C68">
+        <v>6130</v>
+      </c>
+      <c r="D68">
+        <v>1.20820999145507E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69">
+        <v>2048</v>
+      </c>
+      <c r="C69">
+        <v>6174</v>
+      </c>
+      <c r="D69">
+        <v>1.1244058609008701E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70">
+        <v>2048</v>
+      </c>
+      <c r="C70">
+        <v>6170</v>
+      </c>
+      <c r="D70">
+        <v>1.0188102722167899E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71">
+        <v>2048</v>
+      </c>
+      <c r="C71">
+        <v>90546</v>
+      </c>
+      <c r="D71">
+        <v>0.13002896308898901</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72">
+        <v>2048</v>
+      </c>
+      <c r="C72">
+        <v>89128</v>
+      </c>
+      <c r="D72">
+        <v>0.13641691207885701</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73">
+        <v>2048</v>
+      </c>
+      <c r="C73">
+        <v>88097</v>
+      </c>
+      <c r="D73">
+        <v>0.133769035339355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>